<commit_message>
Se actualiza SGDC_DPS2.xlsx: Pruebas de software de Req 06 registrar usuario
</commit_message>
<xml_diff>
--- a/Desarrollo/SGDC/Documentos/DocumentosPruebas/PruebasSoftware/SGDC_DPS2.xlsx
+++ b/Desarrollo/SGDC/Documentos/DocumentosPruebas/PruebasSoftware/SGDC_DPS2.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="8340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="8340" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PSREQ061" sheetId="4" r:id="rId1"/>
-    <sheet name="Notas adicionales" sheetId="11" r:id="rId2"/>
+    <sheet name="PSREQ062" sheetId="12" r:id="rId2"/>
+    <sheet name="Notas adicionales" sheetId="11" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="54">
   <si>
     <t>No</t>
   </si>
@@ -127,6 +128,9 @@
   </si>
   <si>
     <t>Para el campo celular solo debe aceptar numeros, además que los campos de celular y contraseña no acepten espacios</t>
+  </si>
+  <si>
+    <t>El campo usuario aceptar caracteres alfanumericos</t>
   </si>
   <si>
     <t>El boton de Iniciar sesión debe validar si los campos están vacios</t>
@@ -170,7 +174,60 @@
     </r>
   </si>
   <si>
+    <t>PSREQ062</t>
+  </si>
+  <si>
+    <t>Se verifica el codigo y funcionalidad para la pagina de registrar usuario</t>
+  </si>
+  <si>
+    <t>Comprobar el ingreso de datos para registrar usuario</t>
+  </si>
+  <si>
+    <t>Para el campo celular solo debe aceptar numeros, además que los campos no acepten espacios</t>
+  </si>
+  <si>
     <t>El campo celular acepta caracteres alfanumericos</t>
+  </si>
+  <si>
+    <t>El boton de Registrar debe validar si los campos están vacios</t>
+  </si>
+  <si>
+    <t>El boton de Ingresa o Registrate debe abrir la página de iniciar sesión</t>
+  </si>
+  <si>
+    <t>El botón abre la página de iniciar sesión</t>
+  </si>
+  <si>
+    <t>El boton abre la página de iniciar sesión</t>
+  </si>
+  <si>
+    <t>El vinculo Inicia Sesión debe abrir la página de iniciar sesión</t>
+  </si>
+  <si>
+    <t>El vinculo abre la página de iniciar sesión</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Linea 26:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;img src="Recursos/Usuario.jpg"&gt;</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -295,7 +352,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -311,6 +368,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -665,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12:M12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -683,97 +749,97 @@
       <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="10" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="9" t="s">
+      <c r="E2" s="13"/>
+      <c r="F2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9" t="s">
+      <c r="G2" s="12"/>
+      <c r="H2" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="9"/>
+      <c r="I2" s="12"/>
     </row>
     <row r="3" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="13" t="s">
+      <c r="C3" s="15"/>
+      <c r="D3" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="12" t="s">
+      <c r="E3" s="16"/>
+      <c r="F3" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="12"/>
-      <c r="H3" s="14" t="s">
+      <c r="G3" s="15"/>
+      <c r="H3" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="14"/>
+      <c r="I3" s="17"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="15" t="s">
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="16"/>
-      <c r="H4" s="9" t="s">
+      <c r="G4" s="19"/>
+      <c r="H4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="9"/>
+      <c r="I4" s="12"/>
     </row>
     <row r="5" spans="1:14" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="17" t="s">
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="18"/>
-      <c r="H5" s="19">
+      <c r="G5" s="21"/>
+      <c r="H5" s="22">
         <v>45074</v>
       </c>
-      <c r="I5" s="19"/>
+      <c r="I5" s="22"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="20" t="s">
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="21"/>
-      <c r="H7" s="10" t="s">
+      <c r="G7" s="24"/>
+      <c r="H7" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="20" t="s">
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="M7" s="21"/>
+      <c r="M7" s="24"/>
       <c r="N7" s="4" t="s">
         <v>13</v>
       </c>
@@ -782,26 +848,26 @@
       <c r="A8" s="5">
         <v>1</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="22">
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="25">
         <v>45074</v>
       </c>
-      <c r="G8" s="22"/>
-      <c r="H8" s="11" t="s">
+      <c r="G8" s="25"/>
+      <c r="H8" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11" t="s">
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="M8" s="11"/>
+      <c r="M8" s="14"/>
       <c r="N8" s="6" t="s">
         <v>0</v>
       </c>
@@ -810,26 +876,26 @@
       <c r="A9" s="6">
         <v>2</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="22">
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="25">
         <v>45074</v>
       </c>
-      <c r="G9" s="22"/>
-      <c r="H9" s="11" t="s">
+      <c r="G9" s="25"/>
+      <c r="H9" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11" t="s">
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="M9" s="11"/>
+      <c r="M9" s="14"/>
       <c r="N9" s="6" t="s">
         <v>30</v>
       </c>
@@ -838,26 +904,26 @@
       <c r="A10" s="6">
         <v>3</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="22">
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="25">
         <v>45074</v>
       </c>
-      <c r="G10" s="22"/>
-      <c r="H10" s="11" t="s">
+      <c r="G10" s="25"/>
+      <c r="H10" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11" t="s">
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="M10" s="11"/>
+      <c r="M10" s="14"/>
       <c r="N10" s="6" t="s">
         <v>30</v>
       </c>
@@ -866,26 +932,26 @@
       <c r="A11" s="6">
         <v>4</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="22">
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="25">
         <v>45074</v>
       </c>
-      <c r="G11" s="22"/>
-      <c r="H11" s="11" t="s">
+      <c r="G11" s="25"/>
+      <c r="H11" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="M11" s="11"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="M11" s="14"/>
       <c r="N11" s="6" t="s">
         <v>0</v>
       </c>
@@ -894,26 +960,26 @@
       <c r="A12" s="6">
         <v>5</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="22">
+      <c r="B12" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="25">
         <v>45074</v>
       </c>
-      <c r="G12" s="22"/>
-      <c r="H12" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11" t="s">
+      <c r="G12" s="25"/>
+      <c r="H12" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="M12" s="11"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="M12" s="14"/>
       <c r="N12" s="6" t="s">
         <v>30</v>
       </c>
@@ -922,26 +988,26 @@
       <c r="A13" s="7">
         <v>6</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="25">
+        <v>45074</v>
+      </c>
+      <c r="G13" s="25"/>
+      <c r="H13" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="22">
-        <v>45074</v>
-      </c>
-      <c r="G13" s="22"/>
-      <c r="H13" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="M13" s="23"/>
+      <c r="M13" s="26"/>
       <c r="N13" s="7" t="s">
         <v>30</v>
       </c>
@@ -997,10 +1063,376 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="13"/>
+      <c r="F2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="12"/>
+    </row>
+    <row r="3" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="16"/>
+      <c r="F3" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="15"/>
+      <c r="H3" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="17"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="19"/>
+      <c r="H4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="12"/>
+    </row>
+    <row r="5" spans="1:14" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="21"/>
+      <c r="H5" s="22">
+        <v>45074</v>
+      </c>
+      <c r="I5" s="22"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="24"/>
+      <c r="H7" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="M7" s="24"/>
+      <c r="N7" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10">
+        <v>1</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="25">
+        <v>45074</v>
+      </c>
+      <c r="G8" s="25"/>
+      <c r="H8" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="M8" s="14"/>
+      <c r="N8" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="8">
+        <v>2</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="25">
+        <v>45074</v>
+      </c>
+      <c r="G9" s="25"/>
+      <c r="H9" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M9" s="14"/>
+      <c r="N9" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="8">
+        <v>3</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="25">
+        <v>45074</v>
+      </c>
+      <c r="G10" s="25"/>
+      <c r="H10" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M10" s="14"/>
+      <c r="N10" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8">
+        <v>4</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="25">
+        <v>45074</v>
+      </c>
+      <c r="G11" s="25"/>
+      <c r="H11" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="M11" s="14"/>
+      <c r="N11" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="8">
+        <v>5</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="25">
+        <v>45074</v>
+      </c>
+      <c r="G12" s="25"/>
+      <c r="H12" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="M12" s="14"/>
+      <c r="N12" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>6</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="25">
+        <v>45074</v>
+      </c>
+      <c r="G13" s="25"/>
+      <c r="H13" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="M13" s="26"/>
+      <c r="N13" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
+        <v>6</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="25">
+        <v>45074</v>
+      </c>
+      <c r="G14" s="25"/>
+      <c r="H14" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="M14" s="26"/>
+      <c r="N14" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="46">
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1018,63 +1450,101 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="29" t="s">
+      <c r="B2" s="30"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="30"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="26" t="s">
+      <c r="E2" s="33"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="28"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="31"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="12" t="s">
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
+      <c r="A5" s="11" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
+      <c r="A6" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="30"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="33"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="31"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
+      <c r="A7" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J9" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="12">
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:J7"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="G3:J3"/>

</xml_diff>

<commit_message>
Se actualiza SGDC_DPS2.xlsx: Pruebas de software de Req 08 mostrar promociones
</commit_message>
<xml_diff>
--- a/Desarrollo/SGDC/Documentos/DocumentosPruebas/PruebasSoftware/SGDC_DPS2.xlsx
+++ b/Desarrollo/SGDC/Documentos/DocumentosPruebas/PruebasSoftware/SGDC_DPS2.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="8340" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="PSREQ061" sheetId="4" r:id="rId1"/>
     <sheet name="PSREQ062" sheetId="12" r:id="rId2"/>
-    <sheet name="Notas adicionales" sheetId="11" r:id="rId3"/>
+    <sheet name="PSREQ081" sheetId="13" r:id="rId3"/>
+    <sheet name="Notas adicionales" sheetId="11" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="58">
   <si>
     <t>No</t>
   </si>
@@ -228,6 +229,18 @@
       </rPr>
       <t xml:space="preserve"> &lt;img src="Recursos/Usuario.jpg"&gt;</t>
     </r>
+  </si>
+  <si>
+    <t>PSREQ081</t>
+  </si>
+  <si>
+    <t>El botón Elegir debe mostrar mensaje de que ha ordenado el producto</t>
+  </si>
+  <si>
+    <t>Aparece mensaje de haber ordenado el producto con el nombre y precio</t>
+  </si>
+  <si>
+    <t>Se muestra el mensaje con el nombre del producto y precio</t>
   </si>
 </sst>
 </file>
@@ -352,7 +365,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -380,48 +393,75 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -429,24 +469,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -731,7 +753,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -749,97 +771,97 @@
       <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="13" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="12" t="s">
+      <c r="E2" s="18"/>
+      <c r="F2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12" t="s">
+      <c r="G2" s="21"/>
+      <c r="H2" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="12"/>
+      <c r="I2" s="21"/>
     </row>
     <row r="3" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16" t="s">
+      <c r="C3" s="24"/>
+      <c r="D3" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="15" t="s">
+      <c r="E3" s="28"/>
+      <c r="F3" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="17" t="s">
+      <c r="G3" s="24"/>
+      <c r="H3" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="17"/>
+      <c r="I3" s="29"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="18" t="s">
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="19"/>
-      <c r="H4" s="12" t="s">
+      <c r="G4" s="23"/>
+      <c r="H4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="12"/>
+      <c r="I4" s="21"/>
     </row>
     <row r="5" spans="1:14" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="20" t="s">
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="21"/>
-      <c r="H5" s="22">
-        <v>45074</v>
-      </c>
-      <c r="I5" s="22"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="27">
+        <v>45074</v>
+      </c>
+      <c r="I5" s="27"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="23" t="s">
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="24"/>
-      <c r="H7" s="13" t="s">
+      <c r="G7" s="20"/>
+      <c r="H7" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="23" t="s">
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="M7" s="24"/>
+      <c r="M7" s="20"/>
       <c r="N7" s="4" t="s">
         <v>13</v>
       </c>
@@ -848,26 +870,26 @@
       <c r="A8" s="5">
         <v>1</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="25">
-        <v>45074</v>
-      </c>
-      <c r="G8" s="25"/>
-      <c r="H8" s="14" t="s">
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="17">
+        <v>45074</v>
+      </c>
+      <c r="G8" s="17"/>
+      <c r="H8" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14" t="s">
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="M8" s="14"/>
+      <c r="M8" s="16"/>
       <c r="N8" s="6" t="s">
         <v>0</v>
       </c>
@@ -876,26 +898,26 @@
       <c r="A9" s="6">
         <v>2</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="25">
-        <v>45074</v>
-      </c>
-      <c r="G9" s="25"/>
-      <c r="H9" s="14" t="s">
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="17">
+        <v>45074</v>
+      </c>
+      <c r="G9" s="17"/>
+      <c r="H9" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14" t="s">
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="M9" s="14"/>
+      <c r="M9" s="16"/>
       <c r="N9" s="6" t="s">
         <v>30</v>
       </c>
@@ -904,26 +926,26 @@
       <c r="A10" s="6">
         <v>3</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="25">
-        <v>45074</v>
-      </c>
-      <c r="G10" s="25"/>
-      <c r="H10" s="14" t="s">
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="17">
+        <v>45074</v>
+      </c>
+      <c r="G10" s="17"/>
+      <c r="H10" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14" t="s">
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="M10" s="14"/>
+      <c r="M10" s="16"/>
       <c r="N10" s="6" t="s">
         <v>30</v>
       </c>
@@ -932,26 +954,26 @@
       <c r="A11" s="6">
         <v>4</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="25">
-        <v>45074</v>
-      </c>
-      <c r="G11" s="25"/>
-      <c r="H11" s="14" t="s">
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="17">
+        <v>45074</v>
+      </c>
+      <c r="G11" s="17"/>
+      <c r="H11" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14" t="s">
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="M11" s="14"/>
+      <c r="M11" s="16"/>
       <c r="N11" s="6" t="s">
         <v>0</v>
       </c>
@@ -960,26 +982,26 @@
       <c r="A12" s="6">
         <v>5</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="25">
-        <v>45074</v>
-      </c>
-      <c r="G12" s="25"/>
-      <c r="H12" s="14" t="s">
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="17">
+        <v>45074</v>
+      </c>
+      <c r="G12" s="17"/>
+      <c r="H12" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14" t="s">
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="M12" s="14"/>
+      <c r="M12" s="16"/>
       <c r="N12" s="6" t="s">
         <v>30</v>
       </c>
@@ -988,32 +1010,62 @@
       <c r="A13" s="7">
         <v>6</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="25">
-        <v>45074</v>
-      </c>
-      <c r="G13" s="25"/>
-      <c r="H13" s="14" t="s">
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="17">
+        <v>45074</v>
+      </c>
+      <c r="G13" s="17"/>
+      <c r="H13" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="26" t="s">
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="M13" s="26"/>
+      <c r="M13" s="15"/>
       <c r="N13" s="7" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="L10:M10"/>
     <mergeCell ref="L13:M13"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="F13:G13"/>
@@ -1026,6 +1078,612 @@
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="H12:K12"/>
     <mergeCell ref="L12:M12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B2" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="18"/>
+      <c r="F2" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="21"/>
+    </row>
+    <row r="3" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="24"/>
+      <c r="D3" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="28"/>
+      <c r="F3" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="24"/>
+      <c r="H3" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="29"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B4" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="23"/>
+      <c r="H4" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="21"/>
+    </row>
+    <row r="5" spans="1:14" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="26"/>
+      <c r="H5" s="27">
+        <v>45074</v>
+      </c>
+      <c r="I5" s="27"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="20"/>
+      <c r="H7" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="M7" s="20"/>
+      <c r="N7" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10">
+        <v>1</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="17">
+        <v>45074</v>
+      </c>
+      <c r="G8" s="17"/>
+      <c r="H8" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="M8" s="16"/>
+      <c r="N8" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="8">
+        <v>2</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="17">
+        <v>45074</v>
+      </c>
+      <c r="G9" s="17"/>
+      <c r="H9" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="M9" s="16"/>
+      <c r="N9" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="8">
+        <v>3</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="17">
+        <v>45074</v>
+      </c>
+      <c r="G10" s="17"/>
+      <c r="H10" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="M10" s="16"/>
+      <c r="N10" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8">
+        <v>4</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="17">
+        <v>45074</v>
+      </c>
+      <c r="G11" s="17"/>
+      <c r="H11" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="M11" s="16"/>
+      <c r="N11" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="8">
+        <v>5</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="17">
+        <v>45074</v>
+      </c>
+      <c r="G12" s="17"/>
+      <c r="H12" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="M12" s="16"/>
+      <c r="N12" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>6</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="17">
+        <v>45074</v>
+      </c>
+      <c r="G13" s="17"/>
+      <c r="H13" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="M13" s="15"/>
+      <c r="N13" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
+        <v>6</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="17">
+        <v>45074</v>
+      </c>
+      <c r="G14" s="17"/>
+      <c r="H14" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="M14" s="15"/>
+      <c r="N14" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="46">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="L14:M14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11:G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B2" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="18"/>
+      <c r="F2" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="21"/>
+    </row>
+    <row r="3" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="24"/>
+      <c r="D3" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="28"/>
+      <c r="F3" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="24"/>
+      <c r="H3" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="29"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B4" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="23"/>
+      <c r="H4" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="21"/>
+    </row>
+    <row r="5" spans="1:14" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="26"/>
+      <c r="H5" s="27">
+        <v>45074</v>
+      </c>
+      <c r="I5" s="27"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="20"/>
+      <c r="H7" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="M7" s="20"/>
+      <c r="N7" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="13">
+        <v>1</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="17">
+        <v>45074</v>
+      </c>
+      <c r="G8" s="17"/>
+      <c r="H8" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="M8" s="16"/>
+      <c r="N8" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="14">
+        <v>2</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="17">
+        <v>45074</v>
+      </c>
+      <c r="G9" s="17"/>
+      <c r="H9" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="M9" s="16"/>
+      <c r="N9" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="14">
+        <v>3</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="17">
+        <v>45074</v>
+      </c>
+      <c r="G10" s="17"/>
+      <c r="H10" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="M10" s="16"/>
+      <c r="N10" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="14">
+        <v>4</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="17">
+        <v>45074</v>
+      </c>
+      <c r="G11" s="17"/>
+      <c r="H11" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="M11" s="16"/>
+      <c r="N11" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="34">
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="L11:M11"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="H9:K9"/>
@@ -1061,378 +1719,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="8" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="12"/>
-    </row>
-    <row r="3" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="17"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="19"/>
-      <c r="H4" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4" s="12"/>
-    </row>
-    <row r="5" spans="1:14" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="21"/>
-      <c r="H5" s="22">
-        <v>45074</v>
-      </c>
-      <c r="I5" s="22"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="24"/>
-      <c r="H7" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="M7" s="24"/>
-      <c r="N7" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10">
-        <v>1</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="25">
-        <v>45074</v>
-      </c>
-      <c r="G8" s="25"/>
-      <c r="H8" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="M8" s="14"/>
-      <c r="N8" s="8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="8">
-        <v>2</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="25">
-        <v>45074</v>
-      </c>
-      <c r="G9" s="25"/>
-      <c r="H9" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="M9" s="14"/>
-      <c r="N9" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="8">
-        <v>3</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="25">
-        <v>45074</v>
-      </c>
-      <c r="G10" s="25"/>
-      <c r="H10" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="M10" s="14"/>
-      <c r="N10" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8">
-        <v>4</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="25">
-        <v>45074</v>
-      </c>
-      <c r="G11" s="25"/>
-      <c r="H11" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="M11" s="14"/>
-      <c r="N11" s="8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="8">
-        <v>5</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="25">
-        <v>45074</v>
-      </c>
-      <c r="G12" s="25"/>
-      <c r="H12" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="M12" s="14"/>
-      <c r="N12" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7">
-        <v>6</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="25">
-        <v>45074</v>
-      </c>
-      <c r="G13" s="25"/>
-      <c r="H13" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="M13" s="26"/>
-      <c r="N13" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7">
-        <v>6</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="25">
-        <v>45074</v>
-      </c>
-      <c r="G14" s="25"/>
-      <c r="H14" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="M14" s="26"/>
-      <c r="N14" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="46">
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1455,40 +1747,40 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="32" t="s">
+      <c r="B2" s="31"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="33"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="29" t="s">
+      <c r="E2" s="34"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="28" t="s">
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="15" t="s">
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
@@ -1499,58 +1791,58 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="32" t="s">
+      <c r="B6" s="31"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="29" t="s">
+      <c r="E6" s="34"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="32"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="28" t="s">
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="15" t="s">
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J9" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:J2"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="G6:J6"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="G7:J7"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>